<commit_message>
Adjusted Fonts and Edge Case
Commented out in css file for the body to have all Upper Case text.

Added in Roboto from google (bootstrap is overwriting I believe)

Fixed an edge case for which column to display: if the user wants to display all columns which means the player[1] value would be written as undefined in the Winner spreadsheet. This now just leaves a blank string.

Adjusted the modal that displays the sample of rows so that it will "show" after the [readxlsxfile] function has read the file.
</commit_message>
<xml_diff>
--- a/Test Files/raffle-test-data-small.xlsx
+++ b/Test Files/raffle-test-data-small.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vom3-2/Documents/Coding Projects/JS/excel-scroll-winner/Test Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D1FFD4-E940-2A47-9EAB-F7986105E5EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96417BB-D91B-1243-8808-9366A971728C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15840" xr2:uid="{869E327E-0597-49B6-93AA-392FB07B36E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="13">
   <si>
     <t xml:space="preserve">Ben </t>
   </si>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>LastName</t>
-  </si>
-  <si>
-    <t>Ticket</t>
   </si>
 </sst>
 </file>
@@ -429,351 +426,260 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A02D84BE-A8D6-4678-8DE9-29906AAD0543}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>11</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C2">
-        <v>1101021</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3">
-        <v>1101021</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4">
-        <v>1101021</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5">
-        <v>1101021</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C6">
-        <v>1101021</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C7">
-        <v>1101021</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="C8">
-        <v>1101021</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
-      <c r="C9">
-        <v>1101021</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
-      <c r="C10">
-        <v>1101021</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
-      <c r="C11">
-        <v>1101021</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>0</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
       </c>
-      <c r="C12">
-        <v>1101021</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>1</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
       </c>
-      <c r="C13">
-        <v>1101021</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
       </c>
-      <c r="C14">
-        <v>1101021</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>3</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
       </c>
-      <c r="C15">
-        <v>1101021</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>4</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
       </c>
-      <c r="C16">
-        <v>1101021</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>5</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
       </c>
-      <c r="C17">
-        <v>1101021</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>6</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
       </c>
-      <c r="C18">
-        <v>1101021</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>7</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
       </c>
-      <c r="C19">
-        <v>1101021</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>8</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
       </c>
-      <c r="C20">
-        <v>1101021</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>9</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
       </c>
-      <c r="C21">
-        <v>1101021</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>0</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
       </c>
-      <c r="C22">
-        <v>1101021</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>1</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
       </c>
-      <c r="C23">
-        <v>1101021</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>2</v>
       </c>
       <c r="B24" t="s">
         <v>10</v>
       </c>
-      <c r="C24">
-        <v>1101021</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>3</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
       </c>
-      <c r="C25">
-        <v>1101021</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>4</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
       </c>
-      <c r="C26">
-        <v>1101021</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>5</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
       </c>
-      <c r="C27">
-        <v>1101021</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>6</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
       </c>
-      <c r="C28">
-        <v>1101021</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>7</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
       </c>
-      <c r="C29">
-        <v>1101021</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>8</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
       </c>
-      <c r="C30">
-        <v>1101021</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>9</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
-      </c>
-      <c r="C31">
-        <v>1101021</v>
       </c>
     </row>
   </sheetData>
@@ -782,15 +688,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CCED1BDE83DA8B4DB8F8ABBEF203CAA8" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1f6337449571e318062ebe8bb2d569c9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="4b94d919-4f57-4d06-b58c-d7b27c8dab04" xmlns:ns4="f21621c4-57d5-4cdf-80b5-06d6a184f0c3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="756535abd00c106b398a981883d9e6da" ns3:_="" ns4:_="">
     <xsd:import namespace="4b94d919-4f57-4d06-b58c-d7b27c8dab04"/>
@@ -1017,6 +914,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1026,14 +932,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59B5A0F7-783C-4858-B0E3-9275CA8BE5B5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{637BCBDC-C005-477F-A786-DCBBFD4FE0B2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1052,6 +950,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59B5A0F7-783C-4858-B0E3-9275CA8BE5B5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BC1FB7D-B880-478D-B5E2-3979433D4C00}">
   <ds:schemaRefs>

</xml_diff>